<commit_message>
Changed to one scenario
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -19,18 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>G607 DAN</t>
   </si>
 </sst>
 </file>
@@ -348,44 +339,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File with some license plates
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,16 +19,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>G607 DAN</t>
+  </si>
+  <si>
+    <t>MAZDA</t>
+  </si>
+  <si>
+    <t>FV65 ZLZ</t>
+  </si>
+  <si>
+    <t>Y993 PAX</t>
+  </si>
+  <si>
+    <t>Y946 CJW</t>
+  </si>
+  <si>
+    <t>Y736 AKK</t>
+  </si>
+  <si>
+    <t>T62 EVC</t>
+  </si>
+  <si>
+    <t>KIA</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>HONDA</t>
+  </si>
+  <si>
+    <t>BLACK</t>
+  </si>
+  <si>
+    <t>SUZUKI</t>
+  </si>
+  <si>
+    <t>SILVER</t>
+  </si>
+  <si>
+    <t>VAUXHALL</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>License Plate</t>
+  </si>
+  <si>
+    <t>Known Make</t>
+  </si>
+  <si>
+    <t>Known Colour</t>
+  </si>
+  <si>
+    <t>Retrived make</t>
+  </si>
+  <si>
+    <t>Retrived colour</t>
+  </si>
+  <si>
+    <t>PEUGEOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,16 +119,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -81,10 +145,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -119,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -154,7 +218,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -248,21 +312,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -279,7 +343,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -331,28 +395,149 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored to use waits and general improvements to file reading
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>G607 DAN</t>
   </si>
@@ -91,6 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -118,16 +119,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -144,10 +145,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -311,21 +312,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +343,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -394,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -410,11 +411,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -444,6 +445,12 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -455,6 +462,12 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -466,6 +479,12 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -477,6 +496,12 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -488,6 +513,12 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
@@ -499,8 +530,14 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>